<commit_message>
Fixed bug on comm_chest_data spreadsheet; card[3] now pays out $50; previously blank
</commit_message>
<xml_diff>
--- a/Monopoly/Monopoly3.7/comm_chest_data.xlsx
+++ b/Monopoly/Monopoly3.7/comm_chest_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/austinlee/Documents/Python/Personal-Projects/Monopoly/Monopoly3.7/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4F770564-086D-9B49-B48C-E062D358137B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F342ABA-9B8A-4043-A0CF-97C5D4F542D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14360" windowHeight="18000" xr2:uid="{2F7F5140-90C5-7043-97B7-A942DBEC8C1A}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="26">
   <si>
     <t>number</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>upgrades</t>
+  </si>
+  <si>
+    <t>advance</t>
   </si>
 </sst>
 </file>
@@ -462,7 +465,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A18"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -539,6 +542,9 @@
       <c r="C5" t="s">
         <v>20</v>
       </c>
+      <c r="E5">
+        <v>50</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
@@ -554,6 +560,12 @@
       </c>
       <c r="B7" t="s">
         <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7">
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>